<commit_message>
debugged docker-compose,insert mongodb, access mongodb and automatically fill it with basic items
</commit_message>
<xml_diff>
--- a/app/main/assets/db_files/estimator.xlsx
+++ b/app/main/assets/db_files/estimator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
@@ -553,12 +553,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -624,22 +624,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.99"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,7 +838,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="The implementation is based on libsvm. The fit time complexity is more than quadratic with the number of samples which  makes it hard to scale to dataset with more than a couple of 10000 samples.  The multiclass support is handled according to a one-vs-one scheme.  For details on the precise mathematical formulation of the provided kernel functions and how gamma, coef0 and degree  affect each other, see the corresponding section in the narrative documentation: Kernel functions.&#10;&#10;https://scikit-learn.org/stable/modules/generated/sklearn.svm.SVC.html"/>
@@ -856,33 +856,33 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="64.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="60.7448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.6938775510204"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="64.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="60.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.69"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1787,10 +1787,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>